<commit_message>
added data analysis notebook
</commit_message>
<xml_diff>
--- a/Images.xlsx
+++ b/Images.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachid\Desktop\Texas_School_Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C15C55-EE5F-4547-8572-6A5BDF5DC898}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29063BA6-69A2-4DF0-8B9F-7C7C636CFEC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAT-ACT" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Graduated" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -705,15 +704,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:colOff>27215</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>153489</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>391160</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>75475</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -734,8 +733,207 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="342900" y="3208020"/>
-          <a:ext cx="5534660" cy="3451860"/>
+          <a:off x="27215" y="6445432"/>
+          <a:ext cx="5534660" cy="3493226"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>54428</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>119743</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>335782</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>4187</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{529172C3-7ED0-42FD-9E91-51FCB254433D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3102428" y="9002486"/>
+          <a:ext cx="1500554" cy="439615"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Pearson Coefficient: .34</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>64770</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>43544</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>566057</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76202</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3319CA38-4D61-4CA8-868C-4385B040463C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="64770" y="3152504"/>
+          <a:ext cx="2939687" cy="2227218"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>551769</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>185056</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>39769</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69948AE1-BF5E-4279-8B45-EB3021A180ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2990169" y="3886199"/>
+          <a:ext cx="667431" cy="779999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>604158</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>224790</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6211B8A4-647F-439F-9D62-096D44DAA41C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3652158" y="3137536"/>
+          <a:ext cx="2668632" cy="2318384"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -793,50 +991,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>32769</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>84886</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>39369</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AAD81B0-3CC1-4D2D-BAF7-D680B0CB3D35}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="4130636"/>
-          <a:ext cx="5571286" cy="4290733"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>117536</xdr:colOff>
       <xdr:row>29</xdr:row>
@@ -862,7 +1016,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -871,6 +1025,117 @@
         <a:xfrm>
           <a:off x="5603936" y="5427133"/>
           <a:ext cx="1418009" cy="1557118"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>539262</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>169985</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>211016</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>64477</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C681A10-CCB4-403C-A67C-CFDCF2B89341}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3587262" y="3077308"/>
+          <a:ext cx="1500554" cy="439615"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Pearson Coefficient: .45</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>151667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>512100</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>101895</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B1BC0D3-6471-4F5B-8EF5-04DC533E8B7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4314092"/>
+          <a:ext cx="5998500" cy="4293628"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -968,6 +1233,73 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>189914</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>117377</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E1EC971-2FAD-4DD2-B534-A6CE76F68360}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3566160" y="2971800"/>
+          <a:ext cx="1500554" cy="437417"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Pearson Coefficient: .36</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1290,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1308,8 +1640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView topLeftCell="A60" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1326,8 +1658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added participation colenrol visuals
</commit_message>
<xml_diff>
--- a/Images.xlsx
+++ b/Images.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachid\Desktop\Texas_School_Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29063BA6-69A2-4DF0-8B9F-7C7C636CFEC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDDB12C-7A4C-42A5-BEF1-7A6028772876}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAT-ACT" sheetId="1" r:id="rId1"/>
@@ -652,6 +652,228 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>460568</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>151557</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4998AF09-0117-413D-AA0D-51756E7EA868}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="460568" y="5402580"/>
+          <a:ext cx="5460172" cy="4807377"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>453390</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{835B6C18-C469-4238-932A-77A9DB1F0D63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1062990" y="6156960"/>
+          <a:ext cx="1731010" cy="637540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0"/>
+            <a:t>Pearson Coefficient: .48</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>459740</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>100330</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>33020</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48E765F3-F682-4A09-B3E5-512FA5191A89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5946140" y="5440680"/>
+          <a:ext cx="5669280" cy="4795520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14F66CB6-242F-44D2-93DF-EB5D6A94BEB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6445250" y="6172200"/>
+          <a:ext cx="1689100" cy="636270"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>Pearson Coefficient: .52</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1604,8 +1826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1622,7 +1844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
created project deliverables file
</commit_message>
<xml_diff>
--- a/Images.xlsx
+++ b/Images.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachid\Desktop\Texas_School_Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDDB12C-7A4C-42A5-BEF1-7A6028772876}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C97A41-4F10-43B9-A3E7-CD0D4D98D266}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18420" yWindow="2352" windowWidth="8760" windowHeight="6000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAT-ACT" sheetId="1" r:id="rId1"/>
     <sheet name="AP" sheetId="2" r:id="rId2"/>
     <sheet name="Wealth" sheetId="3" r:id="rId3"/>
     <sheet name="Graduated" sheetId="4" r:id="rId4"/>
+    <sheet name="Final Model" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -876,6 +877,48 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C27BBF8A-4A48-4F3E-8A3E-6FF02A87F288}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="657225" y="4838700"/>
+          <a:ext cx="5943600" cy="2324100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1522,6 +1565,99 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>132452</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>106228</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE9E4D35-5027-40F0-B5E4-E87BC28710AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="876300"/>
+          <a:ext cx="7180952" cy="3619048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>168329</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>143184</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{898975CA-192B-4CC6-B3DC-DEE1E83CCC53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6065520" y="1920240"/>
+          <a:ext cx="1418009" cy="1514784"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1826,8 +1962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1844,7 +1980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -1862,8 +1998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1880,7 +2016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
@@ -1892,4 +2028,22 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9707250-8DE8-4D27-90BC-7D6F4DFD5669}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated report and inf statistics
</commit_message>
<xml_diff>
--- a/Images.xlsx
+++ b/Images.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachid\Desktop\Texas_School_Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C97A41-4F10-43B9-A3E7-CD0D4D98D266}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174BE5A7-EDD2-4E35-879E-CDF8E2019C38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18420" yWindow="2352" windowWidth="8760" windowHeight="6000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAT-ACT" sheetId="1" r:id="rId1"/>
@@ -1409,6 +1409,286 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>273039</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>350858</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>170411</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F715D05B-AB59-4298-861B-66EF87ED9B28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="273039" y="12458700"/>
+          <a:ext cx="7393019" cy="4904336"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>279014</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>113262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0F16A81-DE53-4E31-8264-CA9864DBA5D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="279014" y="17354550"/>
+          <a:ext cx="7407661" cy="4837662"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>354044</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>18011</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{307F62B6-A5FB-4E7B-998B-EF899A8B32BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="276225" y="22259925"/>
+          <a:ext cx="7393019" cy="4904336"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41622E0C-8FF0-438D-9BB9-68B380E5B88D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486399" y="26069924"/>
+          <a:ext cx="2324101" cy="676276"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1"/>
+            <a:t>Pearson Coefficient: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1"/>
+            <a:t>.36</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>485776</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7B106B2-0F23-439B-A0BC-3F65A607D913}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5476875" y="20955000"/>
+          <a:ext cx="2324101" cy="676276"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1"/>
+            <a:t>Pearson Coefficient: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1"/>
+            <a:t>.48</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1565,6 +1845,798 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>108857</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>103338</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>201386</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>3531</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{377DAAE6-AC94-442A-B73F-7C75FDC5C326}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="108857" y="8430909"/>
+          <a:ext cx="2530929" cy="2676051"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>185058</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>126063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>255295</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>153221</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDFE7600-0820-4753-A244-0FA189C80B75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2623458" y="8453634"/>
+          <a:ext cx="2508637" cy="2617958"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>326570</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>408213</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>48987</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94802E46-AA29-4FDE-8352-95FA963BA263}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3984170" y="10368643"/>
+          <a:ext cx="1300843" cy="413658"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0"/>
+            <a:t>Pearson Coefficient: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0"/>
+            <a:t>.73</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>201386</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>174170</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>283029</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{286E02A6-0DF0-437D-BBF2-C9D66665AFF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1420586" y="10127795"/>
+          <a:ext cx="1300843" cy="430667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0"/>
+            <a:t>Pearson Coefficient: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0"/>
+            <a:t>.74</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>56266</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>189988</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>61372</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BE5BA8D-5936-43A8-BAEA-30F5AD2C0F27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="56266" y="10906125"/>
+          <a:ext cx="2572122" cy="2728372"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>257176</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>44964</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>475726</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>89944</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DCA202A-BEC5-4B94-8906-428443909A88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2695576" y="10903464"/>
+          <a:ext cx="2656950" cy="2759605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>214312</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A881D63-4B54-4C47-ABBE-18DF2354F1F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="409575" y="11049000"/>
+          <a:ext cx="1023937" cy="528637"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" b="0"/>
+            <a:t>Pearson Coefficient: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" b="0"/>
+            <a:t>.68</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>271462</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BACE9570-E07C-46F3-9262-7FF8E2818DF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4538662" y="12792075"/>
+          <a:ext cx="1023937" cy="528637"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" b="0"/>
+            <a:t>Pearson Coefficient: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" b="0"/>
+            <a:t>.30</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95252</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>59589</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209552</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>85185</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2291191A-05CD-44CD-B21C-5222B0A83CF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="95252" y="13813689"/>
+          <a:ext cx="2552700" cy="2740221"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>433387</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="TextBox 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41421A42-6A31-471F-8712-9DA9F10A4C02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="433387" y="13973175"/>
+          <a:ext cx="852487" cy="519113"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" b="0"/>
+            <a:t>Pearson Coefficient: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" b="0"/>
+            <a:t>.48</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>252414</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>73418</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>89946</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AA0FE54-6AF4-47B6-98D8-2AC29F49A398}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2690814" y="13827518"/>
+          <a:ext cx="2557461" cy="2731153"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>90489</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>123827</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="TextBox 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BA1EAF2-EE90-498D-A9B9-F5815691B05B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3962400" y="14025564"/>
+          <a:ext cx="1371600" cy="395288"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" b="0"/>
+            <a:t>Pearson Coefficient: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" b="0"/>
+            <a:t>.36</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>481013</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>164148</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E7C40FD-B016-4C44-9BC9-75D4B8447C97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="16835438"/>
+          <a:ext cx="2919413" cy="2150110"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>328613</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>547688</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>20003</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{829DDECE-E21A-47FC-90CC-C64329EA7868}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2767013" y="17197388"/>
+          <a:ext cx="1438275" cy="1282065"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1998,8 +3070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView topLeftCell="A124" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="T127" sqref="T127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2016,8 +3088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I100" sqref="I100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>